<commit_message>
update plot for paper
</commit_message>
<xml_diff>
--- a/LIDAR/Results/Data.xlsx
+++ b/LIDAR/Results/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,15 +89,6 @@
   </si>
   <si>
     <t>Exp 3</t>
-  </si>
-  <si>
-    <t>18_09</t>
-  </si>
-  <si>
-    <t>20_09</t>
-  </si>
-  <si>
-    <t>20_10</t>
   </si>
   <si>
     <t>08_04</t>
@@ -230,6 +221,15 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Experiment 1</t>
+  </si>
+  <si>
+    <t>Experiment 2</t>
+  </si>
+  <si>
+    <t>Experiment 3</t>
   </si>
 </sst>
 </file>
@@ -1028,11 +1028,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1272690544"/>
-        <c:axId val="1272691632"/>
+        <c:axId val="-747673056"/>
+        <c:axId val="-747675776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1272690544"/>
+        <c:axId val="-747673056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,7 +1042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1272691632"/>
+        <c:crossAx val="-747675776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1050,7 +1050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1272691632"/>
+        <c:axId val="-747675776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1272690544"/>
+        <c:crossAx val="-747673056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1282,11 +1282,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1272691088"/>
-        <c:axId val="1272688368"/>
+        <c:axId val="-747677408"/>
+        <c:axId val="-747673600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1272691088"/>
+        <c:axId val="-747677408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1272688368"/>
+        <c:crossAx val="-747673600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1304,7 +1304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1272688368"/>
+        <c:axId val="-747673600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1272691088"/>
+        <c:crossAx val="-747677408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1552,11 +1552,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1272688912"/>
-        <c:axId val="1272685648"/>
+        <c:axId val="-747671968"/>
+        <c:axId val="-747676864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1272688912"/>
+        <c:axId val="-747671968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,7 +1566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1272685648"/>
+        <c:crossAx val="-747676864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1574,7 +1574,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1272685648"/>
+        <c:axId val="-747676864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,7 +1585,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1272688912"/>
+        <c:crossAx val="-747671968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1603,6 +1603,733 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.1649910826703375E-2"/>
+          <c:y val="2.2988501964225153E-2"/>
+          <c:w val="0.91676146621110466"/>
+          <c:h val="0.90926140427987656"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>consolidated!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Experiment 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>consolidated!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>consolidated!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2030.1066666666668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1495.7066666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1155.1333333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>628.36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>531.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>289.68666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>234.98666666666671</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.48000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>144.65333333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>162.18666666666664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>consolidated!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Experiment 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>consolidated!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>consolidated!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1704.3913333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476.4246666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1292.7566666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1067.2166666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>767.64400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>209.29173333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>174.56560000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>221.29173333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137.34653333333335</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>107.61173333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>consolidated!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Experiment 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>consolidated!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>consolidated!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1803.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1254.6999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>940.73333333333335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>460.24666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226.65333333333334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107.25333333333334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66.346666666666664</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.733333333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.63333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-747674688"/>
+        <c:axId val="-755163152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-747674688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN" sz="900">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-755163152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-755163152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN" sz="900">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Aerosol Concentration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-747674688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76486850694131492"/>
+          <c:y val="0.15761665538414035"/>
+          <c:w val="0.11542416719242038"/>
+          <c:h val="0.19482175587780035"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1658,11 +2385,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>consolidated!$B$1</c:f>
+              <c:f>consolidated!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>18_09</c:v>
+                  <c:v>08_04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1691,402 +2418,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>consolidated!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>consolidated!$B$2:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2030.1066666666668</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1495.7066666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1155.1333333333334</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>628.36</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>531.54</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>289.68666666666667</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>234.98666666666671</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>176.48000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>144.65333333333334</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>162.18666666666664</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>consolidated!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>20_09</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>consolidated!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>consolidated!$C$2:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1704.3913333333335</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1476.4246666666668</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1292.7566666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1067.2166666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>767.64400000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>209.29173333333335</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>174.56560000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>221.29173333333333</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>137.34653333333335</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>107.61173333333333</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>consolidated!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>20_10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>consolidated!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>consolidated!$D$2:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1803.12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1254.6999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>940.73333333333335</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>460.24666666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>226.65333333333334</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>144.26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>107.25333333333334</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>66.346666666666664</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50.733333333333334</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>66.63333333333334</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>consolidated!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>08_04</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>consolidated!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>consolidated!$E$2:$E$11</c:f>
+              <c:f>consolidated!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2133,11 +2467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1272689456"/>
-        <c:axId val="1272686736"/>
+        <c:axId val="-693713200"/>
+        <c:axId val="-693710480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1272689456"/>
+        <c:axId val="-693713200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2157,7 +2491,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2194,12 +2527,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1272686736"/>
+        <c:crossAx val="-693710480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1272686736"/>
+        <c:axId val="-693710480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1272689456"/>
+        <c:crossAx val="-693713200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2268,38 +2601,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2377,7 +2678,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3008,16 +3865,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3031,6 +3888,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3498,7 +4385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -3510,7 +4397,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -3520,7 +4407,7 @@
       <c r="G1" s="55"/>
       <c r="H1" s="55"/>
       <c r="K1" s="55" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L1" s="55"/>
       <c r="M1" s="55"/>
@@ -3532,52 +4419,52 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="K2" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3585,19 +4472,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -3605,127 +4492,127 @@
         <v>1</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="53"/>
       <c r="B4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K4" s="53"/>
       <c r="L4" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="53"/>
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="K5" s="53"/>
       <c r="L5" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R5" s="8"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K6" s="54"/>
       <c r="L6" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -3733,7 +4620,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -3745,7 +4632,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -3757,7 +4644,7 @@
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -3767,7 +4654,7 @@
       <c r="H8" s="8"/>
       <c r="K8" s="53"/>
       <c r="L8" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -3779,7 +4666,7 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
       <c r="B9" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -3789,7 +4676,7 @@
       <c r="H9" s="8"/>
       <c r="K9" s="53"/>
       <c r="L9" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -3801,7 +4688,7 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="54"/>
       <c r="B10" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -3811,7 +4698,7 @@
       <c r="H10" s="8"/>
       <c r="K10" s="54"/>
       <c r="L10" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -3825,7 +4712,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -3837,7 +4724,7 @@
         <v>3</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -3849,7 +4736,7 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="53"/>
       <c r="B12" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3859,7 +4746,7 @@
       <c r="H12" s="8"/>
       <c r="K12" s="53"/>
       <c r="L12" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -3871,7 +4758,7 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="53"/>
       <c r="B13" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -3881,7 +4768,7 @@
       <c r="H13" s="8"/>
       <c r="K13" s="53"/>
       <c r="L13" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -3893,7 +4780,7 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="54"/>
       <c r="B14" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -3903,7 +4790,7 @@
       <c r="H14" s="8"/>
       <c r="K14" s="54"/>
       <c r="L14" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -3917,7 +4804,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -3929,7 +4816,7 @@
         <v>4</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -3941,7 +4828,7 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
       <c r="B16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -3951,7 +4838,7 @@
       <c r="H16" s="8"/>
       <c r="K16" s="53"/>
       <c r="L16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -3963,7 +4850,7 @@
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
       <c r="B17" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="51"/>
@@ -3973,7 +4860,7 @@
       <c r="H17" s="51"/>
       <c r="K17" s="53"/>
       <c r="L17" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M17" s="51"/>
       <c r="N17" s="51"/>
@@ -3985,7 +4872,7 @@
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
       <c r="B18" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="51"/>
@@ -3995,7 +4882,7 @@
       <c r="H18" s="51"/>
       <c r="K18" s="54"/>
       <c r="L18" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M18" s="51"/>
       <c r="N18" s="51"/>
@@ -4006,16 +4893,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="K3:K6"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="K11:K14"/>
+    <mergeCell ref="K15:K18"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="K3:K6"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="K11:K14"/>
-    <mergeCell ref="K15:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4054,10 +4941,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4105,11 +4992,11 @@
         <v>28.17</v>
       </c>
       <c r="F3" s="49">
-        <f t="shared" ref="F3:F20" si="0">B3-$I$2</f>
+        <f t="shared" ref="F3:F11" si="0">B3-$I$2</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="G3" s="50">
-        <f t="shared" ref="G3:G20" si="1">F3*86400</f>
+        <f t="shared" ref="G3:G11" si="1">F3*86400</f>
         <v>599.99999999999784</v>
       </c>
     </row>
@@ -5402,32 +6289,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5440,11 +6330,11 @@
       <c r="D2">
         <v>1803.12</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>58.55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5457,11 +6347,11 @@
       <c r="D3">
         <v>1254.6999999999998</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="9">
         <v>28.17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5474,11 +6364,11 @@
       <c r="D4">
         <v>940.73333333333335</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="9">
         <v>24.89</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5491,11 +6381,11 @@
       <c r="D5">
         <v>460.24666666666667</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="9">
         <v>22.75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5508,11 +6398,11 @@
       <c r="D6">
         <v>226.65333333333334</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="9">
         <v>23.79</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5525,11 +6415,11 @@
       <c r="D7">
         <v>144.26</v>
       </c>
-      <c r="E7" s="9">
+      <c r="F7" s="9">
         <v>23.85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5542,11 +6432,11 @@
       <c r="D8">
         <v>107.25333333333334</v>
       </c>
-      <c r="E8" s="10">
+      <c r="F8" s="10">
         <v>20.6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5559,11 +6449,11 @@
       <c r="D9">
         <v>66.346666666666664</v>
       </c>
-      <c r="E9" s="11">
+      <c r="F9" s="11">
         <v>21.45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5576,11 +6466,11 @@
       <c r="D10">
         <v>50.733333333333334</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="9">
         <v>20.99</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5593,7 +6483,7 @@
       <c r="D11">
         <v>66.63333333333334</v>
       </c>
-      <c r="E11" s="15">
+      <c r="F11" s="15">
         <v>19.8</v>
       </c>
     </row>
@@ -5621,19 +6511,19 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
       <c r="J1" t="s">
         <v>13</v>
@@ -5661,10 +6551,10 @@
         <v>126.99999999999747</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -5686,10 +6576,10 @@
         <v>246.99999999999704</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5711,7 +6601,7 @@
         <v>367.00000000003979</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K4" s="42">
         <v>0.46895833333333337</v>
@@ -5876,19 +6766,19 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
       <c r="J1" t="s">
         <v>13</v>
@@ -5916,10 +6806,10 @@
         <v>140.00000000000111</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -5941,10 +6831,10 @@
         <v>260.00000000000068</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5991,7 +6881,7 @@
         <v>499.99999999998062</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K5" s="42">
         <v>0.46956018518518516</v>
@@ -6137,25 +7027,25 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>30</v>
-      </c>
       <c r="F1" s="43" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" s="43" t="s">
         <v>13</v>
@@ -6189,10 +7079,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="43" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6220,10 +7110,10 @@
         <v>1</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6282,10 +7172,10 @@
         <v>1</v>
       </c>
       <c r="L5" s="43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -6313,10 +7203,10 @@
         <v>1</v>
       </c>
       <c r="L6" s="43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6344,7 +7234,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M7" s="7">
         <v>0.46388888888888885</v>
@@ -6375,7 +7265,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M8" s="7">
         <v>0.47569444444444442</v>
@@ -6434,7 +7324,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M10" s="44">
         <v>0.4760416666666667</v>

</xml_diff>